<commit_message>
Made graph to pie chart
</commit_message>
<xml_diff>
--- a/Project_File.xlsx
+++ b/Project_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Desktop\School\PYT\Python proj actual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17572966-CA98-4453-8E27-5D3B91004133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A51931-21FB-4DAE-8751-FE3818090544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="2700" windowWidth="17960" windowHeight="10550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="International Monthly Visitor A" sheetId="1" r:id="rId1"/>
@@ -2372,13 +2372,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI480"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="6.7265625" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" customWidth="1"/>
     <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.453125" bestFit="1" customWidth="1"/>

</xml_diff>